<commit_message>
POL-2562: Trucking Inserter Upgrade (#2039)
* POL-2562: initial commit

* POL-2562: almost done

* POL-2562: Trucking Inserter Upgrade

* POL-2562: added backwards compatibility to old load meterage

* POL-2562: fixes for specs

* POL-2562: final linter issues

* POL-2562: comments addressed

Co-authored-by: kodiak-itsmycargo[bot] <80279588+kodiak-itsmycargo[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_trucking.xlsx
+++ b/spec/fixtures/files/excel/example_trucking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
   <si>
     <t>ZONE</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>PERCENTAGE</t>
+  </si>
+  <si>
+    <t>RANGE_MIN</t>
+  </si>
+  <si>
+    <t>RANGE_MAX</t>
   </si>
   <si>
     <t>Fuel Surcharge Fee</t>
@@ -318,6 +324,10 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -330,10 +340,6 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font/>
     <font>
@@ -446,21 +452,24 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -470,19 +479,16 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -2103,42 +2109,48 @@
       <c r="Q1" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="R1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="13">
+      <c r="F2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="14">
         <v>30.0</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -3146,279 +3158,279 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="M1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="N1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="O1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="P1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="Q1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
+      <c r="S1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
     </row>
     <row r="2">
-      <c r="A2" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="18">
+      <c r="A2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="19">
         <v>250.0</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="18">
+      <c r="D2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="19">
         <v>1.0</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="20">
+        <v>44075.0</v>
+      </c>
+      <c r="N2" s="21">
+        <v>44561.0</v>
+      </c>
+      <c r="O2" s="22">
+        <v>1500.0</v>
+      </c>
+      <c r="P2" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>5.0</v>
+      </c>
+      <c r="R2" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="19">
-        <v>44075.0</v>
-      </c>
-      <c r="N2" s="20">
-        <v>44561.0</v>
-      </c>
-      <c r="O2" s="21">
-        <v>1500.0</v>
-      </c>
-      <c r="P2" s="22">
-        <v>8.0</v>
-      </c>
-      <c r="Q2" s="21">
-        <v>5.0</v>
-      </c>
-      <c r="R2" s="21" t="b">
+      <c r="D3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="T2" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="U3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="W3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="X3" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y3" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="D4" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="F4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="G4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="H4" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="I4" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="J4" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="K4" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="L4" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="M4" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="N4" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="O4" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="R4" s="18" t="s">
+      <c r="P4" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="S4" s="18" t="s">
+      <c r="Q4" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="T4" s="18" t="s">
+      <c r="R4" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="U4" s="18" t="s">
+      <c r="S4" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="V4" s="18" t="s">
+      <c r="T4" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="W4" s="18" t="s">
+      <c r="U4" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="V4" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="Y4" s="18" t="s">
+      <c r="W4" s="19" t="s">
         <v>81</v>
+      </c>
+      <c r="X4" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="25">

</xml_diff>

<commit_message>
POL-2826: Finer control for Trucking Fees (#2284)
* starting

* POL-2826: built FeeVersions

* POL-2826: nearly there

* POL-2826: expanding all fees

* POL-2826: generating fees properly

* POL-2826: adding cargo class

* POL-2851: fixed trucking upload through new upload path

* POL-2851: removed pry

* POL-2826: closer and closer

* POL-2826: finally working

* POL-2826: ready to go

* POL-2826: rubocop

* POL-2826: spec fixes

* POL-2826: all specs fixed

* POL-2826: coverage

* POL-2826: removed typo

* POL-2826: rubocop

* POL-2826: comments made and specs fixed

* POL-2826: added guides
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_trucking.xlsx
+++ b/spec/fixtures/files/excel/example_trucking.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Zones" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Fees" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Sheet4" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Zones!$A$1:$D$54</definedName>
@@ -13,14 +14,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mglvSffKQY8KSUMjssDvu2N9yduig=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mgmo0q7QsZ4GeLsMqoBKjtX3/1EPQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="91">
   <si>
     <t>ZONE</t>
   </si>
@@ -34,13 +35,13 @@
     <t>COUNTRY_CODE</t>
   </si>
   <si>
-    <t>20000 - 20050</t>
+    <t>20037 - 20039</t>
   </si>
   <si>
     <t>DE</t>
   </si>
   <si>
-    <t>20051</t>
+    <t>20457</t>
   </si>
   <si>
     <t>FEE</t>
@@ -100,6 +101,15 @@
     <t>RANGE_MAX</t>
   </si>
   <si>
+    <t>CARRIER</t>
+  </si>
+  <si>
+    <t>SERVICE</t>
+  </si>
+  <si>
+    <t>CARGO_CLASS</t>
+  </si>
+  <si>
     <t>Fuel Surcharge Fee</t>
   </si>
   <si>
@@ -121,6 +131,42 @@
     <t>per_shipment</t>
   </si>
   <si>
+    <t>Pickup Fee</t>
+  </si>
+  <si>
+    <t>puf</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>PER_KG</t>
+  </si>
+  <si>
+    <t>Terminal Handling Cost</t>
+  </si>
+  <si>
+    <t>THC</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>PER_SHIPMENT</t>
+  </si>
+  <si>
+    <t>Gateway Cargo GmbH</t>
+  </si>
+  <si>
+    <t>Faster</t>
+  </si>
+  <si>
     <t>CITY</t>
   </si>
   <si>
@@ -136,15 +182,6 @@
     <t>LOAD_TYPE</t>
   </si>
   <si>
-    <t>CARGO_CLASS</t>
-  </si>
-  <si>
-    <t>CARRIER</t>
-  </si>
-  <si>
-    <t>SERVICE</t>
-  </si>
-  <si>
     <t>EFFECTIVE_DATE</t>
   </si>
   <si>
@@ -172,28 +209,13 @@
     <t>Hamburg</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
-    <t>PER_SHIPMENT</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>cargo_item</t>
   </si>
   <si>
     <t>lcl</t>
-  </si>
-  <si>
-    <t>export</t>
-  </si>
-  <si>
-    <t>Gateway Cargo GmbH</t>
   </si>
   <si>
     <t>area</t>
@@ -283,7 +305,7 @@
     <numFmt numFmtId="165" formatCode="yyyy/m/d"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -292,10 +314,6 @@
     <font>
       <b/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <name val="Arial"/>
     </font>
     <font>
@@ -341,7 +359,6 @@
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -417,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -425,13 +442,22 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -439,75 +465,69 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,6 +546,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -744,7 +768,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -755,334 +779,334 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1.0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="6"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="6"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="6"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="6"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="6"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="6"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="6"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="6"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="6"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="6"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="6"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="6"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="6"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="6"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="6"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="6"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="6"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="6"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="3"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="6"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="6"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="6"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1"/>
@@ -2058,99 +2082,172 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="11" t="s">
         <v>25</v>
       </c>
+      <c r="T1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>28</v>
+      <c r="A2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="E2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
       <c r="L2" s="14">
         <v>30.0</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="11">
+        <v>15.0</v>
+      </c>
+      <c r="T3" s="11">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="11">
+        <v>100.0</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
@@ -3154,106 +3251,112 @@
     <col customWidth="1" min="3" max="3" width="20.14"/>
     <col customWidth="1" min="4" max="4" width="28.14"/>
     <col customWidth="1" min="5" max="5" width="22.86"/>
-    <col customWidth="1" min="6" max="26" width="8.86"/>
+    <col customWidth="1" min="6" max="6" width="8.86"/>
+    <col customWidth="1" min="7" max="8" width="12.29"/>
+    <col customWidth="1" min="9" max="9" width="13.71"/>
+    <col customWidth="1" min="10" max="10" width="8.86"/>
+    <col customWidth="1" min="11" max="11" width="19.86"/>
+    <col customWidth="1" min="12" max="12" width="13.29"/>
+    <col customWidth="1" min="13" max="26" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="15" t="s">
+      <c r="A1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="15">
+        <v>250.0</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="16" t="s">
+      <c r="H2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="17" t="s">
+      <c r="K2" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="19">
-        <v>250.0</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="M2" s="20">
         <v>44075.0</v>
@@ -3261,888 +3364,2939 @@
       <c r="N2" s="21">
         <v>44561.0</v>
       </c>
-      <c r="O2" s="22">
+      <c r="O2" s="11">
         <v>1500.0</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="11">
         <v>8.0</v>
       </c>
-      <c r="Q2" s="22">
+      <c r="Q2" s="11">
         <v>5.0</v>
       </c>
-      <c r="R2" s="22" t="b">
+      <c r="R2" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="S2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="Q5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="R5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="S5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="T5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="U5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="V5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="W5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="X5" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="B6" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="26">
+        <v>28.392</v>
+      </c>
+      <c r="D6" s="27">
+        <v>35.49</v>
+      </c>
+      <c r="E6" s="28">
+        <v>45.422</v>
+      </c>
+      <c r="F6" s="27">
+        <v>56.069</v>
+      </c>
+      <c r="G6" s="28">
+        <v>71.69500000000001</v>
+      </c>
+      <c r="H6" s="27">
+        <v>79.495</v>
+      </c>
+      <c r="I6" s="28">
+        <v>88.01</v>
+      </c>
+      <c r="J6" s="27">
+        <v>95.823</v>
+      </c>
+      <c r="K6" s="28">
+        <v>105.05300000000001</v>
+      </c>
+      <c r="L6" s="27">
+        <v>116.40200000000002</v>
+      </c>
+      <c r="M6" s="28">
+        <v>116.4</v>
+      </c>
+      <c r="N6" s="27">
+        <v>117.38749999999999</v>
+      </c>
+      <c r="O6" s="28">
+        <v>121.4875</v>
+      </c>
+      <c r="P6" s="27">
+        <v>127.625</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>131.0375</v>
+      </c>
+      <c r="R6" s="27">
+        <v>134.45</v>
+      </c>
+      <c r="S6" s="28">
+        <v>135.1375</v>
+      </c>
+      <c r="T6" s="27">
+        <v>136.5</v>
+      </c>
+      <c r="U6" s="28">
+        <v>143.325</v>
+      </c>
+      <c r="V6" s="27">
+        <v>147.425</v>
+      </c>
+      <c r="W6" s="28">
+        <v>153.5625</v>
+      </c>
+      <c r="X6" s="27">
+        <v>156.975</v>
+      </c>
+      <c r="Y6" s="28">
+        <v>163.79999999999998</v>
+      </c>
+      <c r="Z6" s="23"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="25"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="23"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="23"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="23"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="23"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="23"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="25"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="23"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="25"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="23"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="25"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="23"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="25"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="23"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="25"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="23"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="25"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="23"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="23"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="25"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="23"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="23"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="25"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="23"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="25"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="23"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="25"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="23"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="25"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="23"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="25"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="23"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="23"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="Z27" s="23"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="2" width="8.86"/>
+    <col customWidth="1" min="3" max="3" width="20.14"/>
+    <col customWidth="1" min="4" max="4" width="28.14"/>
+    <col customWidth="1" min="5" max="5" width="22.86"/>
+    <col customWidth="1" min="6" max="6" width="8.86"/>
+    <col customWidth="1" min="7" max="8" width="12.29"/>
+    <col customWidth="1" min="9" max="9" width="13.71"/>
+    <col customWidth="1" min="10" max="10" width="8.86"/>
+    <col customWidth="1" min="11" max="11" width="19.86"/>
+    <col customWidth="1" min="12" max="12" width="13.29"/>
+    <col customWidth="1" min="13" max="26" width="8.86"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="S1" s="18" t="s">
         <v>59</v>
       </c>
+      <c r="T1" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="15">
+        <v>250.0</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="20">
+        <v>44075.0</v>
+      </c>
+      <c r="N2" s="21">
+        <v>44561.0</v>
+      </c>
+      <c r="O2" s="11">
+        <v>1500.0</v>
+      </c>
+      <c r="P2" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="R2" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3">
-      <c r="C3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="R3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="T3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="W3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="X3" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="19" t="s">
-        <v>51</v>
+      <c r="C3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="D4" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="E4" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="F4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="G4" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="H4" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="P4" s="19" t="s">
+      <c r="I4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="J4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="K4" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="L4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="M4" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="U4" s="19" t="s">
+      <c r="N4" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="V4" s="19" t="s">
+      <c r="O4" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="W4" s="19" t="s">
+      <c r="P4" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="X4" s="19" t="s">
+      <c r="Q4" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Y4" s="19" t="s">
+      <c r="R4" s="15" t="s">
         <v>83</v>
       </c>
+      <c r="S4" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25">
+      <c r="A5" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24">
         <v>0.0</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>0.0</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>0.0</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="24">
         <v>0.0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="24">
         <v>0.0</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="24">
         <v>0.0</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>0.0</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="24">
         <v>0.0</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="24">
         <v>0.0</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="24">
         <v>0.0</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="24">
         <v>0.0</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="24">
         <v>0.0</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="24">
         <v>0.0</v>
       </c>
-      <c r="P5" s="25">
+      <c r="P5" s="24">
         <v>0.0</v>
       </c>
-      <c r="Q5" s="25">
+      <c r="Q5" s="24">
         <v>0.0</v>
       </c>
-      <c r="R5" s="25">
+      <c r="R5" s="24">
         <v>0.0</v>
       </c>
-      <c r="S5" s="25">
+      <c r="S5" s="24">
         <v>0.0</v>
       </c>
-      <c r="T5" s="25">
+      <c r="T5" s="24">
         <v>0.0</v>
       </c>
-      <c r="U5" s="25">
+      <c r="U5" s="24">
         <v>0.0</v>
       </c>
-      <c r="V5" s="25">
+      <c r="V5" s="24">
         <v>0.0</v>
       </c>
-      <c r="W5" s="25">
+      <c r="W5" s="24">
         <v>0.0</v>
       </c>
-      <c r="X5" s="25">
+      <c r="X5" s="24">
         <v>0.0</v>
       </c>
-      <c r="Y5" s="25">
+      <c r="Y5" s="24">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="26">
+      <c r="A6" s="25">
         <v>1.0</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>0.0</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>28.392</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>35.49</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>45.422</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <v>56.069</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>71.69500000000001</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <v>79.495</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="28">
         <v>88.01</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="27">
         <v>95.823</v>
       </c>
-      <c r="K6" s="29">
+      <c r="K6" s="28">
         <v>105.05300000000001</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="27">
         <v>116.40200000000002</v>
       </c>
-      <c r="M6" s="29">
+      <c r="M6" s="28">
         <v>116.4</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="27">
         <v>117.38749999999999</v>
       </c>
-      <c r="O6" s="29">
+      <c r="O6" s="28">
         <v>121.4875</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="27">
         <v>127.625</v>
       </c>
-      <c r="Q6" s="29">
+      <c r="Q6" s="28">
         <v>131.0375</v>
       </c>
-      <c r="R6" s="28">
+      <c r="R6" s="27">
         <v>134.45</v>
       </c>
-      <c r="S6" s="29">
+      <c r="S6" s="28">
         <v>135.1375</v>
       </c>
-      <c r="T6" s="28">
+      <c r="T6" s="27">
         <v>136.5</v>
       </c>
-      <c r="U6" s="29">
+      <c r="U6" s="28">
         <v>143.325</v>
       </c>
-      <c r="V6" s="28">
+      <c r="V6" s="27">
         <v>147.425</v>
       </c>
-      <c r="W6" s="29">
+      <c r="W6" s="28">
         <v>153.5625</v>
       </c>
-      <c r="X6" s="28">
+      <c r="X6" s="27">
         <v>156.975</v>
       </c>
-      <c r="Y6" s="29">
+      <c r="Y6" s="28">
         <v>163.79999999999998</v>
       </c>
-      <c r="Z6" s="24"/>
+      <c r="Z6" s="23"/>
     </row>
     <row r="7">
-      <c r="A7" s="26"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="24"/>
+      <c r="A7" s="32">
+        <v>2.0</v>
+      </c>
+      <c r="B7" s="33">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="29">
+        <f t="shared" ref="C7:Y7" si="1">C6*1.05</f>
+        <v>29.8116</v>
+      </c>
+      <c r="D7" s="29">
+        <f t="shared" si="1"/>
+        <v>37.2645</v>
+      </c>
+      <c r="E7" s="29">
+        <f t="shared" si="1"/>
+        <v>47.6931</v>
+      </c>
+      <c r="F7" s="29">
+        <f t="shared" si="1"/>
+        <v>58.87245</v>
+      </c>
+      <c r="G7" s="29">
+        <f t="shared" si="1"/>
+        <v>75.27975</v>
+      </c>
+      <c r="H7" s="29">
+        <f t="shared" si="1"/>
+        <v>83.46975</v>
+      </c>
+      <c r="I7" s="29">
+        <f t="shared" si="1"/>
+        <v>92.4105</v>
+      </c>
+      <c r="J7" s="29">
+        <f t="shared" si="1"/>
+        <v>100.61415</v>
+      </c>
+      <c r="K7" s="29">
+        <f t="shared" si="1"/>
+        <v>110.30565</v>
+      </c>
+      <c r="L7" s="29">
+        <f t="shared" si="1"/>
+        <v>122.2221</v>
+      </c>
+      <c r="M7" s="29">
+        <f t="shared" si="1"/>
+        <v>122.22</v>
+      </c>
+      <c r="N7" s="29">
+        <f t="shared" si="1"/>
+        <v>123.256875</v>
+      </c>
+      <c r="O7" s="29">
+        <f t="shared" si="1"/>
+        <v>127.561875</v>
+      </c>
+      <c r="P7" s="29">
+        <f t="shared" si="1"/>
+        <v>134.00625</v>
+      </c>
+      <c r="Q7" s="29">
+        <f t="shared" si="1"/>
+        <v>137.589375</v>
+      </c>
+      <c r="R7" s="29">
+        <f t="shared" si="1"/>
+        <v>141.1725</v>
+      </c>
+      <c r="S7" s="29">
+        <f t="shared" si="1"/>
+        <v>141.894375</v>
+      </c>
+      <c r="T7" s="29">
+        <f t="shared" si="1"/>
+        <v>143.325</v>
+      </c>
+      <c r="U7" s="29">
+        <f t="shared" si="1"/>
+        <v>150.49125</v>
+      </c>
+      <c r="V7" s="29">
+        <f t="shared" si="1"/>
+        <v>154.79625</v>
+      </c>
+      <c r="W7" s="29">
+        <f t="shared" si="1"/>
+        <v>161.240625</v>
+      </c>
+      <c r="X7" s="29">
+        <f t="shared" si="1"/>
+        <v>164.82375</v>
+      </c>
+      <c r="Y7" s="29">
+        <f t="shared" si="1"/>
+        <v>171.99</v>
+      </c>
+      <c r="Z7" s="23"/>
     </row>
     <row r="8">
-      <c r="A8" s="26"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="32"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="24"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="23"/>
     </row>
     <row r="9">
-      <c r="A9" s="26"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="31"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="24"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="23"/>
     </row>
     <row r="10">
-      <c r="A10" s="26"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="32"/>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="24"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="23"/>
     </row>
     <row r="11">
-      <c r="A11" s="26"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="31"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="32"/>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="24"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="26"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="32"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="24"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="30"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="30"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="23"/>
     </row>
     <row r="13">
-      <c r="A13" s="26"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="23"/>
     </row>
     <row r="14">
-      <c r="A14" s="26"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="24"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="30"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="23"/>
     </row>
     <row r="15">
-      <c r="A15" s="26"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="31"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="31"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="24"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="30"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="23"/>
     </row>
     <row r="16">
-      <c r="A16" s="26"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="31"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="31"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="31"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="24"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="23"/>
     </row>
     <row r="17">
-      <c r="A17" s="26"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="31"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="24"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="23"/>
     </row>
     <row r="18">
-      <c r="A18" s="26"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="23"/>
     </row>
     <row r="19">
-      <c r="A19" s="26"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="31"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="31"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="32"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="32"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="30"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="23"/>
     </row>
     <row r="20">
-      <c r="A20" s="26"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="29"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="29"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="29"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="29"/>
-      <c r="Z20" s="24"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="23"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="31"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="24"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="30"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="30"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="23"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="32"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="32"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="24"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="31"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="31"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="30"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="30"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="23"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="32"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="24"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="30"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="30"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="23"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="31"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="24"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="23"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="31"/>
-      <c r="Q25" s="32"/>
-      <c r="R25" s="31"/>
-      <c r="S25" s="32"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="32"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="32"/>
-      <c r="X25" s="31"/>
-      <c r="Y25" s="32"/>
-      <c r="Z25" s="24"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="30"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="30"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="23"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="31"/>
-      <c r="S26" s="32"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="32"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="32"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="24"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="23"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="Z27" s="24"/>
+      <c r="Z27" s="23"/>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>

</xml_diff>